<commit_message>
Use of a longer table in more tables
</commit_message>
<xml_diff>
--- a/P3_Ownership.xlsx
+++ b/P3_Ownership.xlsx
@@ -392,19 +392,19 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>140.1379</v>
+        <v>140.1408</v>
       </c>
       <c r="C2" t="n">
-        <v>2114.1399</v>
+        <v>2114.3664</v>
       </c>
       <c r="D2" t="n">
-        <v>130.56</v>
+        <v>141.162</v>
       </c>
       <c r="E2" t="n">
-        <v>68.297</v>
+        <v>69.0453</v>
       </c>
       <c r="F2" t="n">
-        <v>2453.1348</v>
+        <v>2464.7145</v>
       </c>
     </row>
     <row r="3">
@@ -412,19 +412,19 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>47.3219</v>
+        <v>47.3189</v>
       </c>
       <c r="C3" t="n">
-        <v>1079.256</v>
+        <v>1079.0288</v>
       </c>
       <c r="D3" t="n">
-        <v>751.7828</v>
+        <v>741.1805</v>
       </c>
       <c r="E3" t="n">
-        <v>205.608</v>
+        <v>204.8602</v>
       </c>
       <c r="F3" t="n">
-        <v>2083.9687</v>
+        <v>2072.3884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>